<commit_message>
Emociones emitidas por agentes
Emociones emitidas por agentes
</commit_message>
<xml_diff>
--- a/cf_entregable/frames_view.xlsx
+++ b/cf_entregable/frames_view.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guard\Documents\GitHub\html\cf_entregable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\html\cf_entregable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37DCC25-7887-407B-808A-4AA80D59267F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077E9F46-CADD-4E03-B410-7153DFBF8223}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="21181" windowHeight="11402" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="frames_view" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>segmento</t>
   </si>
@@ -73,6 +73,27 @@
   </si>
   <si>
     <t>https://htmlpreview.github.io/?https://raw.githubusercontent.com/DavidIngx/html/master/cf_entregable/afiliaciones_key_words.html</t>
+  </si>
+  <si>
+    <t>whatsapp</t>
+  </si>
+  <si>
+    <t>https://projector.tensorflow.org/?config=https://gist.githubusercontent.com/luiska1803/e65e57239606051a55acecc9753d29d6/raw/d7940b8bcfa124c1f7de469da063bc735e5bd092/Wapp%2520Cafam</t>
+  </si>
+  <si>
+    <t>https://htmlpreview.github.io/?https://github.com/DavidIngx/html/blob/master/cf_entregable/Whatsapp/Palabras_emociones_user.html</t>
+  </si>
+  <si>
+    <t>https://htmlpreview.github.io/?https://github.com/DavidIngx/html/blob/master/cf_entregable/Whatsapp/Experiencia%20General%20User.html</t>
+  </si>
+  <si>
+    <t>https://htmlpreview.github.io/?https://github.com/DavidIngx/html/blob/master/cf_entregable/Whatsapp/Key%20words%20User.html</t>
+  </si>
+  <si>
+    <t>https://htmlpreview.github.io/?https://github.com/DavidIngx/html/blob/master/cf_entregable/Whatsapp/vis_LDA_Chat_wp_usuario.html</t>
+  </si>
+  <si>
+    <t>https://htmlpreview.github.io/?https://github.com/DavidIngx/html/blob/master/cf_entregable/Whatsapp/(N-GRAMAS)_%20User.html</t>
   </si>
 </sst>
 </file>
@@ -401,16 +422,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="150.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -489,6 +510,72 @@
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -499,6 +586,12 @@
     <hyperlink ref="C5" r:id="rId4" xr:uid="{3747812F-84A0-40AA-9D57-F46614C28A6F}"/>
     <hyperlink ref="C6" r:id="rId5" xr:uid="{2EF2B09E-9526-48AD-BC5E-3DE28CEED9D1}"/>
     <hyperlink ref="C7" r:id="rId6" xr:uid="{691B5BD8-E264-41DB-9381-860B55B7B22E}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{1146EE52-BD33-426E-A260-5C5CDD5982DD}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{836C6E02-76B4-4FB5-B0AE-FA42D4355FE9}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{B5A8695A-6414-47CF-B74C-00AFC8D80224}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{09C76CAD-C62E-4480-BDD4-C66A5084D00F}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{F3C7809A-A11A-4BA6-AD98-195B6BD2B96D}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{DD2B5A40-107B-4580-819B-C3509D5C6FF4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>